<commit_message>
Updated for Workspace and added additional codebase
</commit_message>
<xml_diff>
--- a/oscova-excel-bot/OscovaExcelBot/bin/Debug/employees.xlsx
+++ b/oscova-excel-bot/OscovaExcelBot/bin/Debug/employees.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\GitHub\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\GitHub\syn-bot-samples\oscova-excel-bot\OscovaExcelBot\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -459,8 +459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>